<commit_message>
Added determiner functionality for property address
</commit_message>
<xml_diff>
--- a/TestFiles/ExpectedOutput.xlsx
+++ b/TestFiles/ExpectedOutput.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Origami1105\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Origami1105\Source\Repos\BuschEric97\HatcoFilesClosedDeterminer\TestFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27B85E6F-2075-47B5-B11D-AAE1C4EE3536}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEBA34F1-BEDD-4EE7-B5F6-794052354A85}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4500" yWindow="2208" windowWidth="17280" windowHeight="8964" xr2:uid="{B477FE81-BBEC-4E02-88DD-D51E7F5F506A}"/>
+    <workbookView xWindow="18045" yWindow="1680" windowWidth="21600" windowHeight="11385" xr2:uid="{B477FE81-BBEC-4E02-88DD-D51E7F5F506A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -582,19 +582,19 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="14.21875" customWidth="1"/>
-    <col min="5" max="5" width="24.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="14.21875" customWidth="1"/>
-    <col min="10" max="10" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="4" width="14.28515625" customWidth="1"/>
+    <col min="5" max="5" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="14.28515625" customWidth="1"/>
+    <col min="10" max="10" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -626,7 +626,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -658,7 +658,7 @@
         <v>20191011</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -686,11 +686,11 @@
       <c r="I3" s="2">
         <v>135000</v>
       </c>
-      <c r="J3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J3">
+        <v>20191062</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -718,11 +718,11 @@
       <c r="I4" s="2">
         <v>142500</v>
       </c>
-      <c r="J4">
-        <v>20191062</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -754,7 +754,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -786,7 +786,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>36</v>
       </c>
@@ -818,7 +818,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>43</v>
       </c>
@@ -850,7 +850,7 @@
         <v>20190096</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>49</v>
       </c>
@@ -882,7 +882,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -914,7 +914,7 @@
         <v>20182625</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>58</v>
       </c>

</xml_diff>

<commit_message>
Modified logic for match detection
</commit_message>
<xml_diff>
--- a/TestFiles/ExpectedOutput.xlsx
+++ b/TestFiles/ExpectedOutput.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Origami1105\Source\Repos\BuschEric97\HatcoFilesClosedDeterminer\TestFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{941D7BB5-DA82-499B-951E-CA0C74686B13}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A263E14-D8FC-456B-8F46-9BCB1C39A63D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18045" yWindow="1500" windowWidth="21600" windowHeight="11385" xr2:uid="{B477FE81-BBEC-4E02-88DD-D51E7F5F506A}"/>
+    <workbookView xWindow="3660" yWindow="1575" windowWidth="21600" windowHeight="11385" xr2:uid="{B477FE81-BBEC-4E02-88DD-D51E7F5F506A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -591,7 +591,7 @@
     <col min="5" max="5" width="24.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="9" width="14.28515625" customWidth="1"/>
-    <col min="10" max="10" width="11.28515625" customWidth="1"/>
+    <col min="10" max="10" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>